<commit_message>
still bug on url crossinformation
</commit_message>
<xml_diff>
--- a/excel_files_for_testing/presents_list_2.xlsx
+++ b/excel_files_for_testing/presents_list_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u19347\Documents\GitHub\Events-IDF\excel_files_for_testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0C8064-49CD-44E4-BF48-8AF08A78802C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7AAFFC7-740F-4D8C-AD85-0651249EF2BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9225" yWindow="2820" windowWidth="21600" windowHeight="11385" xr2:uid="{2B5C25B3-F4AA-4916-80CA-255E7D923676}"/>
+    <workbookView xWindow="9228" yWindow="2820" windowWidth="21600" windowHeight="11388" xr2:uid="{2B5C25B3-F4AA-4916-80CA-255E7D923676}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון2" sheetId="2" r:id="rId1"/>
@@ -25,18 +25,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>מס אישי</t>
   </si>
   <si>
-    <t>0100</t>
-  </si>
-  <si>
     <t>שם מלא</t>
   </si>
   <si>
-    <t>אור לוינזון</t>
+    <t>010</t>
+  </si>
+  <si>
+    <t>בלה בלה</t>
+  </si>
+  <si>
+    <t>050</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>בלה בלה בלה</t>
+  </si>
+  <si>
+    <t>בלה</t>
   </si>
 </sst>
 </file>
@@ -104,8 +116,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{79333BF0-41C1-4007-BC4C-83507EFD3EAE}" name="טבלה2" displayName="טבלה2" ref="A1:B2" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:B2" xr:uid="{79333BF0-41C1-4007-BC4C-83507EFD3EAE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{79333BF0-41C1-4007-BC4C-83507EFD3EAE}" name="טבלה2" displayName="טבלה2" ref="A1:B4" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:B4" xr:uid="{79333BF0-41C1-4007-BC4C-83507EFD3EAE}"/>
   <tableColumns count="2">
     <tableColumn id="2" xr3:uid="{BB9B93EE-CADD-4559-B978-E4688240F8FB}" name="מס אישי" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{222AF31E-215E-4DC5-A47B-5A4D609DE465}" name="שם מלא" dataDxfId="0"/>
@@ -411,32 +423,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF30302-3142-4475-8778-008E66A4AC6E}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>